<commit_message>
Se creo carpeta de entrega para todo lo realizado en la complementaria de investigación
</commit_message>
<xml_diff>
--- a/04-Sesión/Categorizacion Revistas.xlsx
+++ b/04-Sesión/Categorizacion Revistas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\complementario-3125033\04-Sesion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\complementario-3125033\04-Sesión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2192A0D6-4A42-49AA-8D2C-E7D27293D39A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B84CBD2-1DD3-4E9B-8EDF-853191A522C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D569174F-4A60-4622-86E0-BC10BDE4ABDE}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Nombre Revista</t>
   </si>
@@ -208,6 +208,10 @@
   </si>
   <si>
     <t>Colombia Internacional</t>
+  </si>
+  <si>
+    <t>A traves de la busqueda de revistas en las cuales podria publicar mi artículo, he optado por publicarlo en la revista del SENA, 
+puesto que es mejor y mas facil, ya que al ser parte del SENA tendría acceso directo a recursos y soporte que facilitarían la publicación de mi trabajo, a parte de ser gratis no tendría costos adicionales.</t>
   </si>
 </sst>
 </file>
@@ -312,7 +316,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -352,6 +356,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E7460F-8811-4388-9B15-E2C628D656CC}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -916,7 +926,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -931,6 +941,9 @@
       </c>
       <c r="E12" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1000,6 +1013,9 @@
       <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>